<commit_message>
add provider data code checked in
</commit_message>
<xml_diff>
--- a/InsuranceNow_v1.0/DataDrivenResults/TestResults_1.xlsx
+++ b/InsuranceNow_v1.0/DataDrivenResults/TestResults_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SRajendran\InsuranceNow_v1.0\InsuranceNow_v1.0\DataDrivenResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srajendran\git\seleniumJavaRepo\InsuranceNow_v1.0\DataDrivenResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6D3B6C-E1A2-4727-84E3-13F3414D184F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973DAF9C-BAF1-43CF-9CDB-67DB01A13665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Username</t>
   </si>
@@ -58,43 +58,79 @@
     <t>srajendran</t>
   </si>
   <si>
-    <t>Nov@2024!</t>
-  </si>
-  <si>
-    <t>Jeeva</t>
-  </si>
-  <si>
-    <t>Manor</t>
-  </si>
-  <si>
-    <t>813 544 0847</t>
-  </si>
-  <si>
-    <t>W855744</t>
-  </si>
-  <si>
-    <t>12/31/99</t>
-  </si>
-  <si>
-    <t>JeevaManor@aiiflorida.com</t>
-  </si>
-  <si>
-    <t>Michelle Ivicak</t>
-  </si>
-  <si>
-    <t>Adjuster I</t>
-  </si>
-  <si>
-    <t>CA0LUML</t>
-  </si>
-  <si>
-    <t>Jana</t>
-  </si>
-  <si>
-    <t>JanaManor@aiiflorida.com</t>
-  </si>
-  <si>
-    <t>CA04TZM</t>
+    <t>November@2024!</t>
+  </si>
+  <si>
+    <t>Helen</t>
+  </si>
+  <si>
+    <t>Kebede</t>
+  </si>
+  <si>
+    <t>689 262 7223</t>
+  </si>
+  <si>
+    <t>W854695</t>
+  </si>
+  <si>
+    <t>9/30/27</t>
+  </si>
+  <si>
+    <t>hkebede@ottersolv.com</t>
+  </si>
+  <si>
+    <t>Lesly Dorcely</t>
+  </si>
+  <si>
+    <t>ADJ I</t>
+  </si>
+  <si>
+    <t>CA0QSVC</t>
+  </si>
+  <si>
+    <t>Delonica</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>689 262 7228</t>
+  </si>
+  <si>
+    <t>G183277</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>djames@ottersolv.com</t>
+  </si>
+  <si>
+    <t>Hillary Rape</t>
+  </si>
+  <si>
+    <t>CA0UC2J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashley </t>
+  </si>
+  <si>
+    <t>Hillman</t>
+  </si>
+  <si>
+    <t>689 262 7229</t>
+  </si>
+  <si>
+    <t>W905068</t>
+  </si>
+  <si>
+    <t>ahillman@ottersolv.com</t>
+  </si>
+  <si>
+    <t>Kristal Fisher</t>
+  </si>
+  <si>
+    <t>CA0QQH3</t>
   </si>
 </sst>
 </file>
@@ -105,7 +141,7 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -160,39 +196,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -244,7 +280,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -355,13 +391,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -370,6 +399,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -434,11 +470,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -446,24 +502,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K3"/>
+      <selection activeCell="K2" sqref="K2:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -548,28 +604,63 @@
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
         <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>